<commit_message>
revision 1 uploaded and sent for review
</commit_message>
<xml_diff>
--- a/doc/design/spreadsheets/comparison_matrix_qp.xlsx
+++ b/doc/design/spreadsheets/comparison_matrix_qp.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\MS\doc\design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh\Dropbox\Documents\Thesis\doc\design\spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -175,7 +175,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,61 +219,6 @@
       <b/>
       <i/>
       <sz val="11"/>
-      <color rgb="FF4B0082"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF9F00FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF00FF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFFFF00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF7F00"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -624,13 +569,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -682,6 +620,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -3395,8 +3340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3421,15 +3366,15 @@
       <c r="E1" s="8"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="43" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="50"/>
-      <c r="J1" s="50"/>
-      <c r="K1" s="50"/>
-      <c r="L1" s="50"/>
-      <c r="M1" s="50"/>
-      <c r="N1" s="50"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
       <c r="O1" s="9"/>
       <c r="P1" s="10"/>
     </row>
@@ -3455,31 +3400,31 @@
       <c r="G2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="27">
+      <c r="H2" s="44">
         <v>400</v>
       </c>
-      <c r="I2" s="28">
+      <c r="I2" s="45">
         <v>450</v>
       </c>
-      <c r="J2" s="29">
+      <c r="J2" s="46">
         <v>480</v>
       </c>
-      <c r="K2" s="30">
+      <c r="K2" s="47">
         <v>500</v>
       </c>
-      <c r="L2" s="31">
+      <c r="L2" s="48">
         <v>580</v>
       </c>
-      <c r="M2" s="32">
+      <c r="M2" s="49">
         <v>600</v>
       </c>
-      <c r="N2" s="33">
+      <c r="N2" s="50">
         <v>640</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="P2" s="35" t="s">
+      <c r="P2" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3505,29 +3450,29 @@
       <c r="G3" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="36">
+      <c r="H3" s="29">
         <v>0.14000000000000001</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="30">
         <v>0.19</v>
       </c>
-      <c r="J3" s="38">
+      <c r="J3" s="31">
         <v>0.21</v>
       </c>
-      <c r="K3" s="39">
+      <c r="K3" s="32">
         <v>0.22</v>
       </c>
-      <c r="L3" s="40">
+      <c r="L3" s="33">
         <v>0.31</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M3" s="34">
         <v>0.34499999999999997</v>
       </c>
-      <c r="N3" s="42">
+      <c r="N3" s="35">
         <v>0.4</v>
       </c>
       <c r="O3" s="14"/>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="36" t="s">
         <v>43</v>
       </c>
     </row>
@@ -3575,7 +3520,7 @@
         <v>0.4</v>
       </c>
       <c r="O4" s="18"/>
-      <c r="P4" s="44" t="s">
+      <c r="P4" s="37" t="s">
         <v>15</v>
       </c>
     </row>
@@ -3623,7 +3568,7 @@
         <v>0.4</v>
       </c>
       <c r="O5" s="22"/>
-      <c r="P5" s="45" t="s">
+      <c r="P5" s="38" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3671,7 +3616,7 @@
         <v>0.4</v>
       </c>
       <c r="O6" s="18"/>
-      <c r="P6" s="44" t="s">
+      <c r="P6" s="37" t="s">
         <v>8</v>
       </c>
     </row>
@@ -3721,7 +3666,7 @@
       <c r="O7" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="P7" s="45" t="s">
+      <c r="P7" s="38" t="s">
         <v>18</v>
       </c>
     </row>
@@ -3769,7 +3714,7 @@
         <v>0.45</v>
       </c>
       <c r="O8" s="18"/>
-      <c r="P8" s="44" t="s">
+      <c r="P8" s="37" t="s">
         <v>44</v>
       </c>
     </row>
@@ -3817,7 +3762,7 @@
         <v>0.42</v>
       </c>
       <c r="O9" s="22"/>
-      <c r="P9" s="45" t="s">
+      <c r="P9" s="38" t="s">
         <v>42</v>
       </c>
     </row>
@@ -3865,7 +3810,7 @@
         <v>0.45</v>
       </c>
       <c r="O10" s="18"/>
-      <c r="P10" s="44" t="s">
+      <c r="P10" s="37" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3913,7 +3858,7 @@
         <v>0.42</v>
       </c>
       <c r="O11" s="22"/>
-      <c r="P11" s="45" t="s">
+      <c r="P11" s="38" t="s">
         <v>28</v>
       </c>
     </row>
@@ -3961,54 +3906,54 @@
         <v>0.42</v>
       </c>
       <c r="O12" s="18"/>
-      <c r="P12" s="44" t="s">
+      <c r="P12" s="37" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="46" t="s">
+      <c r="A13" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="47">
+      <c r="B13" s="40">
         <v>156.44</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="48">
+      <c r="D13" s="41">
         <v>633</v>
       </c>
-      <c r="E13" s="47" t="s">
+      <c r="E13" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="48">
+      <c r="F13" s="41">
         <v>24.35</v>
       </c>
-      <c r="G13" s="49" t="s">
+      <c r="G13" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="48">
+      <c r="H13" s="41">
         <v>0.09</v>
       </c>
-      <c r="I13" s="48">
+      <c r="I13" s="41">
         <v>0.18</v>
       </c>
-      <c r="J13" s="48">
+      <c r="J13" s="41">
         <v>0.20499999999999999</v>
       </c>
-      <c r="K13" s="48">
+      <c r="K13" s="41">
         <v>0.22500000000000001</v>
       </c>
-      <c r="L13" s="48">
+      <c r="L13" s="41">
         <v>0.35</v>
       </c>
-      <c r="M13" s="48">
+      <c r="M13" s="41">
         <v>0.38</v>
       </c>
-      <c r="N13" s="48">
+      <c r="N13" s="41">
         <v>0.42</v>
       </c>
-      <c r="O13" s="46" t="s">
+      <c r="O13" s="39" t="s">
         <v>32</v>
       </c>
       <c r="P13" s="26" t="s">

</xml_diff>